<commit_message>
fix listView's tsx config & support hbwElements nest in innerElement & adjust css
</commit_message>
<xml_diff>
--- a/有好货页面/id_1908021/dailyShops/需求表格.xlsx
+++ b/有好货页面/id_1908021/dailyShops/需求表格.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01 repository\01 github\05 geek-fontend\Front-end\有好货页面\id_1908021\dailyShops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D138F49-664B-40A3-885C-1393AC0591C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF25E58-3152-4B58-92FF-DAE66F177C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{280EFB05-5750-C240-B8E3-74A8CB818465}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{280EFB05-5750-C240-B8E3-74A8CB818465}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" activeCellId="1" sqref="E4 E12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -573,7 +573,7 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>